<commit_message>
added first bug to tracker
</commit_message>
<xml_diff>
--- a/Documentation/bugTracker.xlsx
+++ b/Documentation/bugTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanj\Documents\Web Dev Projects\Online Quiz Game\QuizGameAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38322845-B236-4A6A-96D1-084E04F45CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E9EFB0-E5EE-41D5-A243-1845545243F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Bug ID</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>unrecognisable characters in answers</t>
+  </si>
+  <si>
+    <t>On some questions, answers will not display the correct characters as it just displays them in plain text.</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -66,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +85,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,10 +122,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,143 +476,154 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45464</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed an issue with answers and questions being displayed incorrectly. should now display with hthe correct characters.
added some code for being able to add some preferences for future features.
</commit_message>
<xml_diff>
--- a/Documentation/bugTracker.xlsx
+++ b/Documentation/bugTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanj\Documents\Web Dev Projects\Online Quiz Game\QuizGameAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E9EFB0-E5EE-41D5-A243-1845545243F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644F36A8-D92D-4479-8F30-FF64CBC74A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Bug ID</t>
   </si>
@@ -59,7 +59,13 @@
     <t>On some questions, answers will not display the correct characters as it just displays them in plain text.</t>
   </si>
   <si>
-    <t>Ongoing</t>
+    <t>Player name is displayed at the top of the page when game ends</t>
+  </si>
+  <si>
+    <t>When the game finishes, a player name is still displayed at the top of the screen.</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -75,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,12 +91,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,28 +122,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -476,156 +488,185 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="31.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>45464</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="4">
+        <v>45468</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Ongoing">
+      <formula>NOT(ISERROR(SEARCH("Ongoing",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="iconSet" priority="4">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change category and difficulty added
</commit_message>
<xml_diff>
--- a/Documentation/bugTracker.xlsx
+++ b/Documentation/bugTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanj\Documents\Web Dev Projects\Online Quiz Game\QuizGameAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644F36A8-D92D-4479-8F30-FF64CBC74A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E77170-D1B3-47E6-8993-160639648CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
+    <workbookView xWindow="-28905" yWindow="-1680" windowWidth="14610" windowHeight="16305" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Bug ID</t>
   </si>
@@ -53,19 +53,31 @@
     <t>Status</t>
   </si>
   <si>
-    <t>unrecognisable characters in answers</t>
-  </si>
-  <si>
     <t>On some questions, answers will not display the correct characters as it just displays them in plain text.</t>
   </si>
   <si>
-    <t>Player name is displayed at the top of the page when game ends</t>
-  </si>
-  <si>
     <t>When the game finishes, a player name is still displayed at the top of the screen.</t>
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>The game can start even when there are no players added.</t>
+  </si>
+  <si>
+    <t>Player name is displayed at the top of the page when game ends.</t>
+  </si>
+  <si>
+    <t>unrecognisable characters in answers.</t>
+  </si>
+  <si>
+    <t>When the game is started with no players added, no questions are fetched and the finishing leaderboard is displayed.</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Repair Notes</t>
   </si>
 </sst>
 </file>
@@ -90,7 +102,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,20 +139,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -152,6 +164,27 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -485,181 +518,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67E816BD-E648-406C-AF40-E66E5559FF09}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="31.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="2"/>
+    <col min="6" max="6" width="21.26953125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45464</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
-        <v>45464</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45468</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
-        <v>45468</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C4" s="3">
+        <v>45474</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Ongoing">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Ongoing">
       <formula>NOT(ISERROR(SEARCH("Ongoing",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="5">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>

</xml_diff>

<commit_message>
made buttons look nice :)
</commit_message>
<xml_diff>
--- a/Documentation/bugTracker.xlsx
+++ b/Documentation/bugTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanj\Documents\Web Dev Projects\Online Quiz Game\QuizGameAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E77170-D1B3-47E6-8993-160639648CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FAA3B5-DE45-4D94-89DA-F1A2BC794C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28905" yWindow="-1680" windowWidth="14610" windowHeight="16305" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Bug ID</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Repair Notes</t>
+  </si>
+  <si>
+    <t>Added small if statement to check to make sure there is at least one player.</t>
+  </si>
+  <si>
+    <t>Changed all .text to .html and there has been no issues since change.</t>
+  </si>
+  <si>
+    <t>On true or false questions, the answer boxes are too close together.</t>
+  </si>
+  <si>
+    <t>When on a multiple choice question, the answers are too close together.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +164,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -171,20 +183,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -521,7 +519,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +569,9 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
@@ -605,16 +605,28 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45474</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -715,14 +727,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="WIP">
+      <formula>NOT(ISERROR(SEARCH("WIP",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Ongoing">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Ongoing">
       <formula>NOT(ISERROR(SEARCH("Ongoing",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="WIP">
-      <formula>NOT(ISERROR(SEARCH("WIP",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">

</xml_diff>

<commit_message>
added bugs and more to the to-do list.
</commit_message>
<xml_diff>
--- a/Documentation/bugTracker.xlsx
+++ b/Documentation/bugTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanj\Documents\Web Dev Projects\Online Quiz Game\QuizGameAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038D5294-E94E-4848-8FD1-36854EB69CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775D8E9A-BE7D-4113-BF88-DAFEF4DD145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="8270" windowHeight="10170" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5EA7CBB4-F5E0-4957-A3BC-D0BC97F84876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Bug ID</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>&lt;br&gt; tag wasn’t added for one of the answer buttons.</t>
+  </si>
+  <si>
+    <t>First question is not formatted correctly.</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -519,7 +525,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -631,12 +637,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45481</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>